<commit_message>
Impact of Perturbations, Extraction of SubCommunities from excel files
</commit_message>
<xml_diff>
--- a/matrices/Arctic.xlsx
+++ b/matrices/Arctic.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juentz001\Documents\FoodWeb\julia\matrices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juentz001\Documents\FoodWeb\matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE2F563-AD8D-40D1-838D-224CD37F108E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A61882-8429-400D-9BE3-E8EE6AE27223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A4BD88ED-9CD0-4539-BCFD-D4767D3BB142}"/>
   </bookViews>
@@ -21,6 +21,20 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -307,7 +321,7 @@
     </r>
   </si>
   <si>
-    <t>BodyMass of Taxa</t>
+    <t>Primary Producer</t>
   </si>
 </sst>
 </file>
@@ -727,7 +741,7 @@
       <pane xSplit="9" ySplit="14" topLeftCell="BS15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="BX12" sqref="BX12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1152,6 +1166,9 @@
       <c r="BS2">
         <v>137130</v>
       </c>
+      <c r="BU2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="3" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1163,9 +1180,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="BU3" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="BU3" s="1"/>
     </row>
     <row r="4" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1375,6 +1390,10 @@
       <c r="BS4">
         <v>0</v>
       </c>
+      <c r="BU4">
+        <f>SUM(D4:BS4)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1584,6 +1603,10 @@
       <c r="BS5">
         <v>0</v>
       </c>
+      <c r="BU5">
+        <f>SUM(D5:BS5)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1796,6 +1819,10 @@
       <c r="BS6">
         <v>0</v>
       </c>
+      <c r="BU6">
+        <f t="shared" ref="BU6:BU69" si="0">SUM(D6:BS6)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -2007,6 +2034,10 @@
       </c>
       <c r="BS7">
         <v>0</v>
+      </c>
+      <c r="BU7">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:73" x14ac:dyDescent="0.3">
@@ -2220,6 +2251,10 @@
       <c r="BS8">
         <v>0</v>
       </c>
+      <c r="BU8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -2432,6 +2467,10 @@
       <c r="BS9">
         <v>0</v>
       </c>
+      <c r="BU9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -2644,6 +2683,10 @@
       <c r="BS10">
         <v>0</v>
       </c>
+      <c r="BU10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -2856,6 +2899,10 @@
       <c r="BS11">
         <v>0</v>
       </c>
+      <c r="BU11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -3068,6 +3115,10 @@
       <c r="BS12">
         <v>0</v>
       </c>
+      <c r="BU12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -3280,6 +3331,10 @@
       <c r="BS13">
         <v>0</v>
       </c>
+      <c r="BU13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -3492,6 +3547,10 @@
       <c r="BS14">
         <v>0</v>
       </c>
+      <c r="BU14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -3704,6 +3763,10 @@
       <c r="BS15">
         <v>0</v>
       </c>
+      <c r="BU15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -3916,8 +3979,12 @@
       <c r="BS16">
         <v>0</v>
       </c>
+      <c r="BU16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -4128,8 +4195,12 @@
       <c r="BS17">
         <v>0</v>
       </c>
+      <c r="BU17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -4340,8 +4411,12 @@
       <c r="BS18">
         <v>0</v>
       </c>
+      <c r="BU18">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -4552,8 +4627,12 @@
       <c r="BS19">
         <v>0</v>
       </c>
+      <c r="BU19">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -4764,8 +4843,12 @@
       <c r="BS20">
         <v>0</v>
       </c>
+      <c r="BU20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="21" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -4976,8 +5059,12 @@
       <c r="BS21">
         <v>0</v>
       </c>
+      <c r="BU21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="22" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -5188,8 +5275,12 @@
       <c r="BS22">
         <v>0</v>
       </c>
+      <c r="BU22">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -5400,8 +5491,12 @@
       <c r="BS23">
         <v>0</v>
       </c>
+      <c r="BU23">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
     </row>
-    <row r="24" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -5612,8 +5707,12 @@
       <c r="BS24">
         <v>0</v>
       </c>
+      <c r="BU24">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
     </row>
-    <row r="25" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -5824,8 +5923,12 @@
       <c r="BS25">
         <v>0</v>
       </c>
+      <c r="BU25">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
     </row>
-    <row r="26" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -6036,8 +6139,12 @@
       <c r="BS26">
         <v>0</v>
       </c>
+      <c r="BU26">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
     </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -6248,8 +6355,12 @@
       <c r="BS27">
         <v>0</v>
       </c>
+      <c r="BU27">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
     </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -6460,8 +6571,12 @@
       <c r="BS28">
         <v>0</v>
       </c>
+      <c r="BU28">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -6672,8 +6787,12 @@
       <c r="BS29">
         <v>0</v>
       </c>
+      <c r="BU29">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -6884,8 +7003,12 @@
       <c r="BS30">
         <v>0</v>
       </c>
+      <c r="BU30">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="31" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -7096,8 +7219,12 @@
       <c r="BS31">
         <v>0</v>
       </c>
+      <c r="BU31">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="32" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -7308,8 +7435,12 @@
       <c r="BS32">
         <v>0</v>
       </c>
+      <c r="BU32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -7520,8 +7651,12 @@
       <c r="BS33">
         <v>0</v>
       </c>
+      <c r="BU33">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
     </row>
-    <row r="34" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -7732,8 +7867,12 @@
       <c r="BS34">
         <v>0</v>
       </c>
+      <c r="BU34">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
     </row>
-    <row r="35" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -7944,8 +8083,12 @@
       <c r="BS35">
         <v>0</v>
       </c>
+      <c r="BU35">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
     </row>
-    <row r="36" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -8156,8 +8299,12 @@
       <c r="BS36">
         <v>0</v>
       </c>
+      <c r="BU36">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
     </row>
-    <row r="37" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -8368,8 +8515,12 @@
       <c r="BS37">
         <v>0</v>
       </c>
+      <c r="BU37">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
     </row>
-    <row r="38" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -8580,8 +8731,12 @@
       <c r="BS38">
         <v>0</v>
       </c>
+      <c r="BU38">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
     </row>
-    <row r="39" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -8792,8 +8947,12 @@
       <c r="BS39">
         <v>0</v>
       </c>
+      <c r="BU39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -9004,8 +9163,12 @@
       <c r="BS40">
         <v>0</v>
       </c>
+      <c r="BU40">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="41" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -9216,8 +9379,12 @@
       <c r="BS41">
         <v>0</v>
       </c>
+      <c r="BU41">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="42" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -9428,8 +9595,12 @@
       <c r="BS42">
         <v>0</v>
       </c>
+      <c r="BU42">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="43" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -9640,8 +9811,12 @@
       <c r="BS43">
         <v>0</v>
       </c>
+      <c r="BU43">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="44" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -9852,8 +10027,12 @@
       <c r="BS44">
         <v>0</v>
       </c>
+      <c r="BU44">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="45" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -10064,8 +10243,12 @@
       <c r="BS45">
         <v>0</v>
       </c>
+      <c r="BU45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="46" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -10276,8 +10459,12 @@
       <c r="BS46">
         <v>0</v>
       </c>
+      <c r="BU46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -10488,8 +10675,12 @@
       <c r="BS47">
         <v>0</v>
       </c>
+      <c r="BU47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -10700,8 +10891,12 @@
       <c r="BS48">
         <v>0</v>
       </c>
+      <c r="BU48">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="49" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -10912,8 +11107,12 @@
       <c r="BS49">
         <v>0</v>
       </c>
+      <c r="BU49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="50" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>32</v>
       </c>
@@ -11124,8 +11323,12 @@
       <c r="BS50">
         <v>0</v>
       </c>
+      <c r="BU50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>33</v>
       </c>
@@ -11333,8 +11536,12 @@
       <c r="BS51">
         <v>0</v>
       </c>
+      <c r="BU51">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
     </row>
-    <row r="52" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>34</v>
       </c>
@@ -11542,8 +11749,12 @@
       <c r="BS52">
         <v>0</v>
       </c>
+      <c r="BU52">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
     </row>
-    <row r="53" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>35</v>
       </c>
@@ -11751,8 +11962,12 @@
       <c r="BS53">
         <v>0</v>
       </c>
+      <c r="BU53">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
     </row>
-    <row r="54" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -11963,8 +12178,12 @@
       <c r="BS54">
         <v>0</v>
       </c>
+      <c r="BU54">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
     </row>
-    <row r="55" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -12175,8 +12394,12 @@
       <c r="BS55">
         <v>0</v>
       </c>
+      <c r="BU55">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
     </row>
-    <row r="56" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -12387,8 +12610,12 @@
       <c r="BS56">
         <v>0</v>
       </c>
+      <c r="BU56">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="57" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>39</v>
       </c>
@@ -12599,8 +12826,12 @@
       <c r="BS57">
         <v>0</v>
       </c>
+      <c r="BU57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>40</v>
       </c>
@@ -12811,8 +13042,12 @@
       <c r="BS58">
         <v>0</v>
       </c>
+      <c r="BU58">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="59" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>41</v>
       </c>
@@ -13023,8 +13258,12 @@
       <c r="BS59">
         <v>0</v>
       </c>
+      <c r="BU59">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
     </row>
-    <row r="60" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -13235,8 +13474,12 @@
       <c r="BS60">
         <v>0</v>
       </c>
+      <c r="BU60">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -13447,8 +13690,12 @@
       <c r="BS61">
         <v>0</v>
       </c>
+      <c r="BU61">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
     </row>
-    <row r="62" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -13659,8 +13906,12 @@
       <c r="BS62">
         <v>0</v>
       </c>
+      <c r="BU62">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
     </row>
-    <row r="63" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>42</v>
       </c>
@@ -13871,8 +14122,12 @@
       <c r="BS63">
         <v>0</v>
       </c>
+      <c r="BU63">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
     </row>
-    <row r="64" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>66</v>
       </c>
@@ -14080,8 +14335,12 @@
       <c r="BS64">
         <v>0</v>
       </c>
+      <c r="BU64">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="65" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -14286,8 +14545,12 @@
       <c r="BS65">
         <v>0</v>
       </c>
+      <c r="BU65">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
-    <row r="66" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -14499,8 +14762,12 @@
       <c r="BS66">
         <v>0</v>
       </c>
+      <c r="BU66">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
     </row>
-    <row r="67" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -14712,8 +14979,12 @@
       <c r="BS67">
         <v>0</v>
       </c>
+      <c r="BU67">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="68" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -14922,8 +15193,12 @@
       <c r="BS68">
         <v>0</v>
       </c>
+      <c r="BU68">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="69" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>71</v>
       </c>
@@ -15135,8 +15410,12 @@
       <c r="BS69">
         <v>0</v>
       </c>
+      <c r="BU69">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="70" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>72</v>
       </c>
@@ -15345,8 +15624,12 @@
       <c r="BS70">
         <v>0</v>
       </c>
+      <c r="BU70">
+        <f t="shared" ref="BU70:BU71" si="1">SUM(D70:BS70)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="71" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>73</v>
       </c>
@@ -15557,6 +15840,10 @@
       </c>
       <c r="BS71">
         <v>0</v>
+      </c>
+      <c r="BU71">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>